<commit_message>
Update the DELETE_MARKE from "X" to "1.0" the same like a funcElec Concept
</commit_message>
<xml_diff>
--- a/de.dlr.sc.virsat.model.extension.budget.cost.test/resources/CostTypeCollectionTest.xlsx
+++ b/de.dlr.sc.virsat.model.extension.budget.cost.test/resources/CostTypeCollectionTest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\VirtualSatellite4-Core\de.dlr.sc.virsat.model.extension.budget.cost.test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6EA84C2-08C1-47B5-9CBD-521B219B46B7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{289E1559-E159-47FB-BF7F-5251BDE382F4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="108" windowWidth="20112" windowHeight="9528" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
   <si>
     <t xml:space="preserve"> Structural Element UUID</t>
   </si>
@@ -118,9 +118,6 @@
   </si>
   <si>
     <t>Test</t>
-  </si>
-  <si>
-    <t>X</t>
   </si>
 </sst>
 </file>
@@ -986,8 +983,8 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B8" s="1" t="s">
-        <v>32</v>
+      <c r="B8" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>